<commit_message>
almost finished bootstrapping everything
</commit_message>
<xml_diff>
--- a/planif.xlsx
+++ b/planif.xlsx
@@ -162,9 +162,6 @@
     <t>Réalisation &amp; recherche</t>
   </si>
   <si>
-    <t>Présentation Oauth 2 le 02.03.18. Continuation sur l'implémentation oauth en php</t>
-  </si>
-  <si>
     <t>Présentation &amp; réalisation</t>
   </si>
   <si>
@@ -184,6 +181,9 @@
   </si>
   <si>
     <t>Avoir une liste de scope qui sa'ffiche pour aider les utilisateurs de la plateforme. Avoir un mechanisme d'authentification permettant d'être délié d'un système d'authentification</t>
+  </si>
+  <si>
+    <t>Présentation Oauth 2 le 28.02.18. Continuation sur l'implémentation oauth en php</t>
   </si>
 </sst>
 </file>
@@ -355,47 +355,8 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -414,27 +375,66 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,7 +722,7 @@
   <dimension ref="A1:DL32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8:J8"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -739,13 +739,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:116" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="36"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="4" t="s">
         <v>0</v>
       </c>
@@ -758,16 +758,16 @@
         <v>2</v>
       </c>
       <c r="I1" s="4"/>
-      <c r="J1" s="35"/>
+      <c r="J1" s="17"/>
     </row>
     <row r="2" spans="1:116" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33">
+      <c r="A2" s="18">
         <v>5</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="34">
         <v>43129</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="31">
         <v>43133</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -783,13 +783,13 @@
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:116" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="15"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
@@ -802,8 +802,8 @@
         <v>10</v>
       </c>
       <c r="I3" s="5"/>
-      <c r="J3" s="35" t="s">
-        <v>51</v>
+      <c r="J3" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -913,13 +913,13 @@
       <c r="DL3" s="2"/>
     </row>
     <row r="4" spans="1:116" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33">
+      <c r="A4" s="18">
         <v>6</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="36">
         <v>43136</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="29">
         <v>43140</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -935,7 +935,7 @@
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1045,9 +1045,9 @@
       <c r="DL4" s="2"/>
     </row>
     <row r="5" spans="1:116" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="15"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1060,8 +1060,8 @@
         <v>12</v>
       </c>
       <c r="I5" s="5"/>
-      <c r="J5" s="35" t="s">
-        <v>51</v>
+      <c r="J5" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1171,13 +1171,13 @@
       <c r="DL5" s="2"/>
     </row>
     <row r="6" spans="1:116" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33">
+      <c r="A6" s="18">
         <v>7</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6" s="36">
         <v>43143</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="29">
         <v>43147</v>
       </c>
       <c r="D6" s="3" t="s">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1303,9 +1303,9 @@
       <c r="DL6" s="2"/>
     </row>
     <row r="7" spans="1:116" s="4" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="14"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
@@ -1315,11 +1315,11 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="35" t="s">
-        <v>51</v>
+      <c r="J7" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1429,24 +1429,24 @@
       <c r="DL7" s="2"/>
     </row>
     <row r="8" spans="1:116" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34">
+      <c r="A8" s="16">
         <v>8</v>
       </c>
-      <c r="B8" s="27">
+      <c r="B8" s="14">
         <v>43150</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="15">
         <v>43154</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="J8" s="30"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="22"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
@@ -1555,13 +1555,13 @@
       <c r="DL8" s="2"/>
     </row>
     <row r="9" spans="1:116" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="33">
+      <c r="A9" s="18">
         <v>9</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="32">
         <v>43157</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="31">
         <v>43161</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -1569,7 +1569,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1687,11 +1687,11 @@
       <c r="DL9" s="2"/>
     </row>
     <row r="10" spans="1:116" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="15"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
@@ -1699,11 +1699,11 @@
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="I10" s="5"/>
-      <c r="J10" s="35" t="s">
-        <v>51</v>
+      <c r="J10" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1813,13 +1813,13 @@
       <c r="DL10" s="2"/>
     </row>
     <row r="11" spans="1:116" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="31">
+      <c r="A11" s="20">
         <v>10</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="32">
         <v>43164</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="31">
         <v>43168</v>
       </c>
       <c r="D11" s="3" t="s">
@@ -1835,7 +1835,7 @@
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1945,9 +1945,9 @@
       <c r="DL11" s="2"/>
     </row>
     <row r="12" spans="1:116" s="4" customFormat="1" ht="69.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="15"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="5" t="s">
         <v>45</v>
       </c>
@@ -1960,8 +1960,8 @@
         <v>15</v>
       </c>
       <c r="I12" s="5"/>
-      <c r="J12" s="35" t="s">
-        <v>51</v>
+      <c r="J12" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -2071,13 +2071,13 @@
       <c r="DL12" s="2"/>
     </row>
     <row r="13" spans="1:116" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="33">
+      <c r="A13" s="18">
         <v>11</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="32">
         <v>43171</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="31">
         <v>43175</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -2203,9 +2203,9 @@
       <c r="DL13" s="2"/>
     </row>
     <row r="14" spans="1:116" s="4" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="15"/>
+      <c r="A14" s="19"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="30"/>
       <c r="D14" s="5" t="s">
         <v>44</v>
       </c>
@@ -2218,8 +2218,8 @@
         <v>21</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="35" t="s">
-        <v>51</v>
+      <c r="J14" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -2329,13 +2329,13 @@
       <c r="DL14" s="2"/>
     </row>
     <row r="15" spans="1:116" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
+      <c r="A15" s="18">
         <v>12</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="32">
         <v>43178</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="31">
         <v>43182</v>
       </c>
       <c r="D15" s="3" t="s">
@@ -2351,7 +2351,7 @@
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -2461,9 +2461,9 @@
       <c r="DL15" s="2"/>
     </row>
     <row r="16" spans="1:116" s="4" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="19"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="30"/>
       <c r="D16" s="5" t="s">
         <v>44</v>
       </c>
@@ -2476,8 +2476,8 @@
         <v>22</v>
       </c>
       <c r="I16" s="5"/>
-      <c r="J16" s="35" t="s">
-        <v>51</v>
+      <c r="J16" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -2587,13 +2587,13 @@
       <c r="DL16" s="2"/>
     </row>
     <row r="17" spans="1:116" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31">
+      <c r="A17" s="20">
         <v>13</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="32">
         <v>43185</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="31">
         <v>43189</v>
       </c>
       <c r="D17" s="3" t="s">
@@ -2609,7 +2609,7 @@
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -2719,9 +2719,9 @@
       <c r="DL17" s="2"/>
     </row>
     <row r="18" spans="1:116" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="31"/>
       <c r="D18" s="3" t="s">
         <v>43</v>
       </c>
@@ -2734,8 +2734,8 @@
         <v>23</v>
       </c>
       <c r="I18" s="5"/>
-      <c r="J18" s="35" t="s">
-        <v>51</v>
+      <c r="J18" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -2845,24 +2845,24 @@
       <c r="DL18" s="2"/>
     </row>
     <row r="19" spans="1:116" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
+      <c r="A19" s="18">
         <v>14</v>
       </c>
-      <c r="B19" s="20">
+      <c r="B19" s="9">
         <v>43192</v>
       </c>
-      <c r="C19" s="24">
+      <c r="C19" s="11">
         <v>43196</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="18"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="24"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
@@ -2971,20 +2971,20 @@
       <c r="DL19" s="2"/>
     </row>
     <row r="20" spans="1:116" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="26">
+      <c r="A20" s="19"/>
+      <c r="B20" s="13">
         <v>43199</v>
       </c>
-      <c r="C20" s="25">
+      <c r="C20" s="12">
         <v>43203</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="22"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="25"/>
+      <c r="I20" s="25"/>
+      <c r="J20" s="26"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -3093,16 +3093,16 @@
       <c r="DL20" s="2"/>
     </row>
     <row r="21" spans="1:116" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="31">
+      <c r="A21" s="20">
         <v>15</v>
       </c>
-      <c r="B21" s="12">
+      <c r="B21" s="32">
         <v>43206</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="34">
         <v>43210</v>
       </c>
-      <c r="D21" s="23" t="s">
+      <c r="D21" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E21" s="2"/>
@@ -3115,7 +3115,7 @@
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -3225,10 +3225,10 @@
       <c r="DL21" s="2"/>
     </row>
     <row r="22" spans="1:116" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="19" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="5" t="s">
@@ -3239,8 +3239,8 @@
         <v>39</v>
       </c>
       <c r="I22" s="5"/>
-      <c r="J22" s="35" t="s">
-        <v>51</v>
+      <c r="J22" s="17" t="s">
+        <v>50</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -4435,6 +4435,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="D8:J8"/>
@@ -4451,21 +4466,6 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="60" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>